<commit_message>
Almost part 1 is done
the part KPIs of ENV are mostly done.
and the unit handling as well.
</commit_message>
<xml_diff>
--- a/exs/eee.xlsx
+++ b/exs/eee.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0a02c4a7808a1f27/Desktop/newStuff/Danalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0a02c4a7808a1f27/Desktop/newStuff/Danalysis/exs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="5" documentId="11_A8F58CBAFFBC04F54BA611124940CC774C9F23E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6B7A323-1B2C-4E48-B4AD-CDEAF89C6C1D}"/>
@@ -12832,6 +12832,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13136,8 +13140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1724" sqref="B1724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>